<commit_message>
vylepšena funkcionalita přidat kod, pohodlnější obsluha
</commit_message>
<xml_diff>
--- a/temporary.xlsx
+++ b/temporary.xlsx
@@ -1,44 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Desktop\rostlinolekarske_pasy\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FC0FD5-5C1E-4615-8A9E-721B6A12DC5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5085" yWindow="5535" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5085" yWindow="5535" windowWidth="28800" windowHeight="15345" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="List1" sheetId="1" r:id="rId1"/>
+    <sheet name="List1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -46,26 +41,92 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -331,14 +392,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="3" max="3" width="48.7109375" customWidth="1"/>
+    <col width="48.7109375" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>